<commit_message>
Added the Signup and Signin tests
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="testData" sheetId="1" r:id="rId1"/>
+    <sheet name="signup_data" sheetId="1" r:id="rId1"/>
+    <sheet name="signin_data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>email</t>
   </si>
@@ -38,7 +39,7 @@
     <t>isValid</t>
   </si>
   <si>
-    <t>user@example.com</t>
+    <t>user5@example.com</t>
   </si>
   <si>
     <t>ValidPass@123</t>
@@ -699,7 +700,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -714,6 +715,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1250,8 +1257,8 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1307,12 +1314,80 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="user@example.com" tooltip="mailto:user@example.com"/>
-    <hyperlink ref="A4" r:id="rId2" display="another@example.com" tooltip="mailto:another@example.com"/>
-    <hyperlink ref="B2" r:id="rId3" display="ValidPass@123"/>
+    <hyperlink ref="A2" r:id="rId1" display="user5@example.com" tooltip="mailto:user5@example.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="ValidPass@123"/>
+    <hyperlink ref="A4" r:id="rId3" display="another@example.com" tooltip="mailto:another@example.com"/>
     <hyperlink ref="B3" r:id="rId4" display="Short@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="17.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3">
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="user5@example.com" tooltip="mailto:user5@example.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="ValidPass@123"/>
+    <hyperlink ref="B3" r:id="rId3" display="Short@123"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up tracked files after .gitignore update
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>isValid</t>
   </si>
   <si>
-    <t>user5@example.com</t>
+    <t>user10@example.com</t>
   </si>
   <si>
     <t>ValidPass@123</t>
@@ -710,10 +710,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1257,8 +1257,8 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1280,42 +1280,42 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="b">
+      <c r="C2" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="b">
+      <c r="C3" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="b">
+      <c r="C4" s="4" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="user5@example.com" tooltip="mailto:user5@example.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="ValidPass@123"/>
+    <hyperlink ref="A2" r:id="rId1" display="user10@example.com" tooltip="mailto:user10@example.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
     <hyperlink ref="A4" r:id="rId3" display="another@example.com" tooltip="mailto:another@example.com"/>
     <hyperlink ref="B3" r:id="rId4" display="Short@123"/>
   </hyperlinks>
@@ -1329,8 +1329,8 @@
   <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -1355,21 +1355,21 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="b">
+      <c r="C2" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="b">
+      <c r="C3" s="4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1383,9 +1383,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="user5@example.com" tooltip="mailto:user5@example.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="ValidPass@123"/>
-    <hyperlink ref="B3" r:id="rId3" display="Short@123"/>
+    <hyperlink ref="B2" r:id="rId1" display="ValidPass@123"/>
+    <hyperlink ref="B3" r:id="rId2" display="Short@123"/>
+    <hyperlink ref="A2" r:id="rId3" display="user10@example.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Clean up untracked files from Git index
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>email</t>
   </si>
@@ -39,22 +39,29 @@
     <t>isValid</t>
   </si>
   <si>
-    <t>user11@example.com</t>
+    <t>rohan.kapse.iic.0148+RockStar@gmail.com</t>
   </si>
   <si>
     <t>ValidPass@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rohan.kapse.iic.0148+RockStar2@gmail.com
+</t>
+  </si>
+  <si>
+    <t>another@example.com</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>user11@example.com</t>
   </si>
   <si>
     <t>user@</t>
   </si>
   <si>
     <t>Short@123</t>
-  </si>
-  <si>
-    <t>another@example.com</t>
-  </si>
-  <si>
-    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -700,7 +707,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -721,6 +728,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1257,13 +1267,13 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="33.3333333333333" customWidth="1"/>
     <col min="2" max="2" width="17.8888888888889" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
@@ -1279,7 +1289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" ht="28.8" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1290,23 +1300,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+    <row r="3" ht="43.2" spans="1:3">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>0</v>
@@ -1314,10 +1324,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="user11@example.com" tooltip="mailto:user11@example.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
-    <hyperlink ref="A4" r:id="rId3" display="another@example.com" tooltip="mailto:another@example.com"/>
-    <hyperlink ref="B3" r:id="rId4" display="Short@123"/>
+    <hyperlink ref="B2" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="A4" r:id="rId2" display="another@example.com" tooltip="mailto:another@example.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="rohan.kapse.iic.0148+RockStar2@gmail.com&#10;"/>
+    <hyperlink ref="B3" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1329,8 +1339,8 @@
   <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -1353,7 +1363,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -1364,10 +1374,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Add the test and chatpage file for Chat Test
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
     <sheet name="signin_data" sheetId="2" r:id="rId2"/>
+    <sheet name="chatTest_Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>email</t>
   </si>
@@ -62,6 +63,51 @@
   </si>
   <si>
     <t>Short@123</t>
+  </si>
+  <si>
+    <t>CreatorEmail</t>
+  </si>
+  <si>
+    <t>CreatorPassword</t>
+  </si>
+  <si>
+    <t>FanEmail1</t>
+  </si>
+  <si>
+    <t>FanEmail2</t>
+  </si>
+  <si>
+    <t>FanEmail3</t>
+  </si>
+  <si>
+    <t>MessageType</t>
+  </si>
+  <si>
+    <t>MessageContent</t>
+  </si>
+  <si>
+    <t>rohankapse520@gmail.com</t>
+  </si>
+  <si>
+    <t>Rohan@2025</t>
+  </si>
+  <si>
+    <t>rohan.kapse@iiclab.com</t>
+  </si>
+  <si>
+    <t>rohankapse45@gmail.com</t>
+  </si>
+  <si>
+    <t>rohan.kapse.iic.0148+RockStart@gmail.com</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Hello from Excel!</t>
+  </si>
+  <si>
+    <t>./media/test-image.jpg</t>
   </si>
 </sst>
 </file>
@@ -74,12 +120,28 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -100,14 +162,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -436,7 +490,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -445,16 +499,136 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -577,150 +751,183 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -729,7 +936,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1267,7 +1474,7 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1278,47 +1485,47 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="12" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="b">
+      <c r="C2" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="b">
+      <c r="C3" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="b">
+      <c r="C4" s="14" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1350,46 +1557,46 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="12" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="b">
+      <c r="C2" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="b">
+      <c r="C3" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="5"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1400,4 +1607,110 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="36.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="27.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="19.1111111111111" customWidth="1"/>
+    <col min="4" max="4" width="19.8888888888889" customWidth="1"/>
+    <col min="5" max="5" width="22.7777777777778" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="28.3333333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" ht="40" customHeight="1" spans="1:7">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" ht="44" customHeight="1" spans="1:7">
+      <c r="A3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId4" display="rohan.kapse.iic.0148+RockStart@gmail.com" tooltip="mailto:fan3@example.com"/>
+    <hyperlink ref="A3" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId5" display="Rohan@2025"/>
+    <hyperlink ref="C3" r:id="rId2" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
+    <hyperlink ref="D3" r:id="rId3" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId4" display="rohan.kapse.iic.0148+RockStart@gmail.com" tooltip="mailto:fan3@example.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added and update the massMessageTest file and Chatpage.js
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
     <sheet name="signin_data" sheetId="2" r:id="rId2"/>
-    <sheet name="chatTest_Data" sheetId="3" r:id="rId3"/>
+    <sheet name="massMsgSend_Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>email</t>
   </si>
@@ -71,15 +71,6 @@
     <t>CreatorPassword</t>
   </si>
   <si>
-    <t>FanEmail1</t>
-  </si>
-  <si>
-    <t>FanEmail2</t>
-  </si>
-  <si>
-    <t>FanEmail3</t>
-  </si>
-  <si>
     <t>MessageType</t>
   </si>
   <si>
@@ -92,22 +83,10 @@
     <t>Rohan@2025</t>
   </si>
   <si>
-    <t>rohan.kapse@iiclab.com</t>
-  </si>
-  <si>
-    <t>rohankapse45@gmail.com</t>
-  </si>
-  <si>
-    <t>rohan.kapse.iic.0148+RockStart@gmail.com</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Hello from Excel!</t>
-  </si>
-  <si>
-    <t>./media/test-image.jpg</t>
+    <t>media</t>
+  </si>
+  <si>
+    <t>C:\Users\Himani\Pictures\image5.jpeg</t>
   </si>
 </sst>
 </file>
@@ -139,6 +118,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -160,14 +147,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -490,72 +469,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -569,66 +488,6 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -751,13 +610,13 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -769,34 +628,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -881,63 +740,48 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1485,47 +1329,47 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="13" t="s">
+    <row r="1" s="11" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14" t="b">
+      <c r="C2" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="b">
+      <c r="C3" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="14" t="b">
+      <c r="C4" s="4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1557,46 +1401,46 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="13" t="s">
+    <row r="1" s="11" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14" t="b">
+      <c r="C2" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="14" t="b">
+      <c r="C3" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="16"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1612,25 +1456,25 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="36.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="27.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="19.1111111111111" customWidth="1"/>
-    <col min="4" max="4" width="19.8888888888889" customWidth="1"/>
-    <col min="5" max="5" width="22.7777777777778" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="28.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="35.5555555555556" customWidth="1"/>
+    <col min="5" max="5" width="22.7777777777778" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28.3333333333333" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1642,73 +1486,52 @@
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
       <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
-      <c r="A3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
-    <hyperlink ref="D2" r:id="rId3" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
-    <hyperlink ref="E2" r:id="rId4" display="rohan.kapse.iic.0148+RockStart@gmail.com" tooltip="mailto:fan3@example.com"/>
-    <hyperlink ref="A3" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId5" display="Rohan@2025"/>
-    <hyperlink ref="C3" r:id="rId2" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
-    <hyperlink ref="D3" r:id="rId3" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
-    <hyperlink ref="E3" r:id="rId4" display="rohan.kapse.iic.0148+RockStart@gmail.com" tooltip="mailto:fan3@example.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Rohan@2025"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add and Upadate massMessageTest file for Creator and Fan Users
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
     <sheet name="signin_data" sheetId="2" r:id="rId2"/>
     <sheet name="massMsgSend_Data" sheetId="3" r:id="rId3"/>
+    <sheet name="users_LoginData" sheetId="4" r:id="rId4"/>
+    <sheet name="massMessageTest_Flow" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>email</t>
   </si>
@@ -71,22 +73,43 @@
     <t>CreatorPassword</t>
   </si>
   <si>
-    <t>MessageType</t>
-  </si>
-  <si>
-    <t>MessageContent</t>
-  </si>
-  <si>
     <t>rohankapse520@gmail.com</t>
   </si>
   <si>
     <t>Rohan@2025</t>
   </si>
   <si>
-    <t>media</t>
-  </si>
-  <si>
-    <t>C:\Users\Himani\Pictures\image5.jpeg</t>
+    <t>FanEmail</t>
+  </si>
+  <si>
+    <t>FanPassword</t>
+  </si>
+  <si>
+    <t>rohan.kapse@iiclab.com</t>
+  </si>
+  <si>
+    <t>Rohan@001</t>
+  </si>
+  <si>
+    <t>rohankapse45@gmail.com</t>
+  </si>
+  <si>
+    <t>Test Details for Send the MassMessage Feature</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">massMessageTest  &gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Login As Creator then Send the Message to All followers and All Active Subscribers. Then login as fan and navigate to chat then verify that message is recived or not.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -740,33 +763,42 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1329,14 +1361,14 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="14" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1344,7 +1376,7 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="b">
@@ -1355,7 +1387,7 @@
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4" t="b">
@@ -1401,14 +1433,14 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="14" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1416,7 +1448,7 @@
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="b">
@@ -1427,7 +1459,7 @@
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="4" t="b">
@@ -1435,12 +1467,12 @@
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="6"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1458,8 +1490,8 @@
   <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1468,72 +1500,159 @@
     <col min="2" max="2" width="27.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="19.1111111111111" customWidth="1"/>
     <col min="4" max="4" width="35.5555555555556" customWidth="1"/>
-    <col min="5" max="5" width="22.7777777777778" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.3333333333333" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7777777777778" style="8" customWidth="1"/>
+    <col min="6" max="6" width="20" style="8" customWidth="1"/>
+    <col min="7" max="7" width="28.3333333333333" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
-      <c r="A3" s="4"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="6"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
     <hyperlink ref="B2" r:id="rId2" display="Rohan@2025"/>
+    <hyperlink ref="A3" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="Rohan@2025"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="46.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="26.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="28" customHeight="1" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" ht="31" customHeight="1" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:2">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
+    <hyperlink ref="A3" r:id="rId3" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId4" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="B4" r:id="rId4" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="48.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" ht="57.6" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added the fan test and chatwithCreator method
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -85,19 +85,27 @@
     <t>FanPassword</t>
   </si>
   <si>
+    <t>rohankapse45@gmail.com</t>
+  </si>
+  <si>
     <t>rohan.kapse@iiclab.com</t>
   </si>
   <si>
     <t>Rohan@001</t>
   </si>
   <si>
-    <t>rohankapse45@gmail.com</t>
-  </si>
-  <si>
     <t>Test Details for Send the MassMessage Feature</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">massMessageTest  &gt;&gt; </t>
     </r>
     <r>
@@ -141,15 +149,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -633,10 +641,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
@@ -777,16 +785,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1373,35 +1381,35 @@
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="b">
+      <c r="C2" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="b">
+      <c r="C3" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="b">
+      <c r="C4" s="6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1445,24 +1453,24 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="b">
+      <c r="C2" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="b">
+      <c r="C3" s="6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1519,27 +1527,27 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="10"/>
       <c r="F2" s="11"/>
       <c r="G2" s="10"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="10"/>
       <c r="F3" s="11"/>
       <c r="G3" s="10"/>
@@ -1573,7 +1581,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1592,35 +1600,35 @@
     </row>
     <row r="2" ht="28" customHeight="1" spans="1:2">
       <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" ht="31" customHeight="1" spans="1:2">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:2">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" ht="31" customHeight="1" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" ht="30" customHeight="1" spans="1:2">
-      <c r="A4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
+    <hyperlink ref="A4" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
+    <hyperlink ref="B4" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
     <hyperlink ref="A3" r:id="rId3" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
     <hyperlink ref="B3" r:id="rId4" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
-    <hyperlink ref="B4" r:id="rId4" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="B2" r:id="rId4" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update the ChatPage and massMessageTest
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="3"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>email</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>FanPassword</t>
-  </si>
-  <si>
-    <t>rohankapse45@gmail.com</t>
   </si>
   <si>
     <t>rohan.kapse@iiclab.com</t>
@@ -118,6 +115,9 @@
       </rPr>
       <t>Login As Creator then Send the Message to All followers and All Active Subscribers. Then login as fan and navigate to chat then verify that message is recived or not.</t>
     </r>
+  </si>
+  <si>
+    <t>rohankapse45@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -781,9 +781,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -791,6 +788,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1381,13 +1381,13 @@
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="b">
+      <c r="C2" s="5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1395,21 +1395,21 @@
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="b">
+      <c r="C3" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="b">
+      <c r="C4" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1453,24 +1453,24 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="b">
+      <c r="C2" s="5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="b">
+      <c r="C3" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1499,7 +1499,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1514,40 +1514,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="10"/>
       <c r="F2" s="11"/>
       <c r="G2" s="10"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
-      <c r="A3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="10"/>
       <c r="F3" s="11"/>
       <c r="G3" s="10"/>
@@ -1567,8 +1563,6 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
     <hyperlink ref="B2" r:id="rId2" display="Rohan@2025"/>
-    <hyperlink ref="A3" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="Rohan@2025"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1580,8 +1574,8 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1591,44 +1585,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" ht="28" customHeight="1" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" ht="31" customHeight="1" spans="1:2">
-      <c r="A3" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" ht="30" customHeight="1" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    </row>
+    <row r="3" ht="31" customHeight="1"/>
+    <row r="4" ht="30" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
-    <hyperlink ref="B4" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
-    <hyperlink ref="A3" r:id="rId3" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId4" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
-    <hyperlink ref="B2" r:id="rId4" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="A2" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1638,28 +1615,49 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="48.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" ht="57.6" spans="1:1">
       <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" ht="28.8" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" ht="28.8" spans="1:2">
+      <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A10" r:id="rId1" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
+    <hyperlink ref="B10" r:id="rId2" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="B9" r:id="rId2" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Add the getLastRecivedMsgCreator() and update fan test
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="4"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -1359,7 +1359,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1431,7 +1431,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -1499,7 +1499,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1574,8 +1574,8 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1615,13 +1615,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="48.5555555555556" customWidth="1"/>
   </cols>
@@ -1636,27 +1636,27 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" ht="28.8" spans="1:2">
-      <c r="A9" s="3" t="s">
+    <row r="5" ht="28.8" spans="1:2">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" ht="28.8" spans="1:2">
-      <c r="A10" s="5" t="s">
+    <row r="6" ht="28.8" spans="1:2">
+      <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
-    <hyperlink ref="B10" r:id="rId2" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
-    <hyperlink ref="B9" r:id="rId2" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="A6" r:id="rId1" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
+    <hyperlink ref="B6" r:id="rId2" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="B5" r:id="rId2" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update the getmsgrecived method
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="3"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>email</t>
   </si>
@@ -1498,8 +1498,8 @@
   <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1540,14 +1540,26 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
-      <c r="A3" s="5"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="10"/>
       <c r="F3" s="11"/>
       <c r="G3" s="10"/>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="5" spans="1:2">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
@@ -1563,6 +1575,10 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
     <hyperlink ref="B2" r:id="rId2" display="Rohan@2025"/>
+    <hyperlink ref="A3" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="Rohan@2025"/>
+    <hyperlink ref="B4" r:id="rId2" display="Rohan@2025"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1574,8 +1590,8 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1600,12 +1616,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" ht="31" customHeight="1"/>
-    <row r="4" ht="30" customHeight="1"/>
+    <row r="3" ht="31" customHeight="1" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:2">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
     <hyperlink ref="B2" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
+    <hyperlink ref="A3" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
+    <hyperlink ref="A4" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
+    <hyperlink ref="B4" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Delete unused waitChatToLoad method
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>email</t>
   </si>
@@ -1499,7 +1499,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1540,12 +1540,8 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="10"/>
@@ -1553,12 +1549,8 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="12"/>
@@ -1575,10 +1567,6 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
     <hyperlink ref="B2" r:id="rId2" display="Rohan@2025"/>
-    <hyperlink ref="A3" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
-    <hyperlink ref="A4" r:id="rId1" display="rohankapse520@gmail.com" tooltip="mailto:rohankapse520@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="Rohan@2025"/>
-    <hyperlink ref="B4" r:id="rId2" display="Rohan@2025"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1591,7 +1579,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1617,29 +1605,17 @@
       </c>
     </row>
     <row r="3" ht="31" customHeight="1" spans="1:2">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:2">
-      <c r="A4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
     <hyperlink ref="B2" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
-    <hyperlink ref="A3" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
-    <hyperlink ref="A4" r:id="rId1" display="rohan.kapse@iiclab.com" tooltip="mailto:rohan.kapse@iiclab.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
-    <hyperlink ref="B4" r:id="rId2" display="Rohan@001" tooltip="mailto:Rohan@001"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1652,7 +1628,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
Added the generatePhrase method
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -1498,7 +1498,7 @@
   <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1578,8 +1578,8 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1628,7 +1628,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
Updated the flow of masstest and fan msg verify test
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="3"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>email</t>
   </si>
@@ -73,10 +73,16 @@
     <t>CreatorPassword</t>
   </si>
   <si>
+    <t>MessageType</t>
+  </si>
+  <si>
     <t>rohankapse520@gmail.com</t>
   </si>
   <si>
     <t>Rohan@2025</t>
+  </si>
+  <si>
+    <t>Creator</t>
   </si>
   <si>
     <t>FanEmail</t>
@@ -771,7 +777,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -799,14 +805,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1369,14 +1387,14 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="15" t="s">
+    <row r="1" s="18" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1441,14 +1459,14 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="15" t="s">
+    <row r="1" s="18" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1475,12 +1493,12 @@
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="10"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1498,8 +1516,8 @@
   <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1520,48 +1538,50 @@
       <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="C1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
       <c r="A3" s="5"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="14"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" s="13"/>
+      <c r="B7" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1578,8 +1598,8 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1590,18 +1610,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" ht="28" customHeight="1" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" ht="31" customHeight="1" spans="1:2">
@@ -1638,12 +1658,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" ht="57.6" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" ht="28.8" spans="1:2">
@@ -1656,7 +1676,7 @@
     </row>
     <row r="6" ht="28.8" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
update the data file
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>email</t>
   </si>
@@ -76,19 +76,22 @@
     <t>MessageType</t>
   </si>
   <si>
+    <t>ImagePath</t>
+  </si>
+  <si>
     <t>rohankapse520@gmail.com</t>
   </si>
   <si>
     <t>Rohan@2025</t>
   </si>
   <si>
-    <t>Creator</t>
-  </si>
-  <si>
     <t>FanEmail</t>
   </si>
   <si>
     <t>FanPassword</t>
+  </si>
+  <si>
+    <t>Message Type</t>
   </si>
   <si>
     <t>rohan.kapse@iiclab.com</t>
@@ -506,7 +509,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -521,6 +524,19 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -653,7 +669,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -665,34 +681,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -777,7 +793,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -799,9 +815,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -811,22 +839,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1387,14 +1406,14 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="18" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="19" t="s">
+    <row r="1" s="19" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1410,7 +1429,7 @@
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1459,14 +1478,14 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="18" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="19" t="s">
+    <row r="1" s="19" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1493,12 +1512,12 @@
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="12"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1516,8 +1535,8 @@
   <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1526,9 +1545,8 @@
     <col min="2" max="2" width="27.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="19.1111111111111" customWidth="1"/>
     <col min="4" max="4" width="35.5555555555556" customWidth="1"/>
-    <col min="5" max="5" width="22.7777777777778" style="8" customWidth="1"/>
-    <col min="6" max="6" width="20" style="8" customWidth="1"/>
-    <col min="7" max="7" width="28.3333333333333" style="8" customWidth="1"/>
+    <col min="5" max="5" width="20" style="12" customWidth="1"/>
+    <col min="7" max="7" width="28.3333333333333" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1538,50 +1556,54 @@
       <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="D1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="12"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
       <c r="A3" s="5"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="14"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="B3" s="9"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="5"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" s="17"/>
+      <c r="B7" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1596,41 +1618,53 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="46.3333333333333" customWidth="1"/>
     <col min="2" max="2" width="26.5555555555556" customWidth="1"/>
+    <col min="3" max="3" width="20.4444444444444" customWidth="1"/>
+    <col min="4" max="4" width="18.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" ht="28" customHeight="1" spans="1:2">
+      <c r="C1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" ht="28" customHeight="1" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" ht="31" customHeight="1" spans="1:2">
+      <c r="B2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" ht="31" customHeight="1" spans="1:4">
       <c r="A3" s="5"/>
-      <c r="B3" s="7"/>
-    </row>
-    <row r="4" ht="30" customHeight="1" spans="1:2">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" ht="30" customHeight="1" spans="1:4">
       <c r="A4" s="5"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1648,7 +1682,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
@@ -1658,12 +1692,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="57.6" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" ht="28.8" spans="1:2">
@@ -1676,7 +1710,7 @@
     </row>
     <row r="6" ht="28.8" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Added new test for negative test and po class for nagative test
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="3"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
     <sheet name="signin_data" sheetId="2" r:id="rId2"/>
     <sheet name="massMsgSend_Data" sheetId="3" r:id="rId3"/>
     <sheet name="users_LoginData" sheetId="4" r:id="rId4"/>
-    <sheet name="massMessageTest_Flow" sheetId="5" r:id="rId5"/>
+    <sheet name="massMessage_TestScenarios" sheetId="5" r:id="rId5"/>
+    <sheet name="massVaultMedia_TestScenarios" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>email</t>
   </si>
@@ -42,13 +43,13 @@
     <t>isValid</t>
   </si>
   <si>
-    <t>rohan.kapse.iic.0148+RockStar@gmail.com</t>
+    <t>rohan.kapse.iic.0148+RockHero@gmail.com</t>
   </si>
   <si>
     <t>ValidPass@123</t>
   </si>
   <si>
-    <t xml:space="preserve">rohan.kapse.iic.0148+RockStar2@gmail.com
+    <t xml:space="preserve">rohan.kapse.iic.0148+RockStar3@gmail.com
 </t>
   </si>
   <si>
@@ -126,7 +127,46 @@
     </r>
   </si>
   <si>
+    <t>rohan.kapse.iic.0148+RockStar@gmail.com</t>
+  </si>
+  <si>
     <t>rohankapse45@gmail.com</t>
+  </si>
+  <si>
+    <t>Mass Media Vault Recived Feature by Fan/User</t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
+  </si>
+  <si>
+    <t>Test Scenarios</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postive </t>
+  </si>
+  <si>
+    <t>a. Fan recived the Sended vault media files and pay for it.</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>a. Creator without vault media files.</t>
+  </si>
+  <si>
+    <t>Mass Media Vault Send Feature by Creator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. Creator Send vault media files </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. Creator without vault media files </t>
   </si>
 </sst>
 </file>
@@ -149,6 +189,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -172,14 +220,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -663,12 +703,12 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -793,50 +833,59 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -845,16 +894,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1396,7 +1442,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1406,47 +1452,47 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="19" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="20" t="s">
+    <row r="1" s="21" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="b">
+      <c r="C2" s="11" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="b">
+      <c r="C3" s="11" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="b">
+      <c r="C4" s="11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1454,7 +1500,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
     <hyperlink ref="A4" r:id="rId2" display="another@example.com" tooltip="mailto:another@example.com"/>
-    <hyperlink ref="A3" r:id="rId3" display="rohan.kapse.iic.0148+RockStar2@gmail.com&#10;"/>
+    <hyperlink ref="A3" r:id="rId3" display="rohan.kapse.iic.0148+RockStar3@gmail.com&#10;"/>
     <hyperlink ref="B3" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1468,7 +1514,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
@@ -1478,46 +1524,46 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="19" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="20" t="s">
+    <row r="1" s="21" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="b">
+      <c r="C2" s="11" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="b">
+      <c r="C3" s="11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="16"/>
+      <c r="C4" s="19"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1536,7 +1582,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="6"/>
@@ -1545,65 +1591,65 @@
     <col min="2" max="2" width="27.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="19.1111111111111" customWidth="1"/>
     <col min="4" max="4" width="35.5555555555556" customWidth="1"/>
-    <col min="5" max="5" width="20" style="12" customWidth="1"/>
-    <col min="7" max="7" width="28.3333333333333" style="12" customWidth="1"/>
+    <col min="5" max="5" width="20" style="16" customWidth="1"/>
+    <col min="7" max="7" width="28.3333333333333" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="14"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="G2" s="16"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
-      <c r="A3" s="5"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="15"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
-      <c r="G3" s="16"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="15"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="15"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" s="18"/>
+      <c r="B7" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1620,8 +1666,8 @@
   <sheetPr/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -1633,37 +1679,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="8"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" ht="28" customHeight="1" spans="1:4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="11"/>
     </row>
     <row r="3" ht="31" customHeight="1" spans="1:4">
-      <c r="A3" s="5"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="11"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="11"/>
     </row>
   </sheetData>
@@ -1679,44 +1725,137 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="48.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="9.88888888888889" customWidth="1"/>
+    <col min="2" max="2" width="49.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="26.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" ht="57.6" spans="1:1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" ht="28.8" spans="1:2">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" ht="28.8" spans="1:2">
-      <c r="A6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="11" ht="15.6" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="4">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:D11"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" display="rohankapse45@gmail.com" tooltip="mailto:rohankapse45@gmail.com"/>
     <hyperlink ref="B6" r:id="rId2" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
@@ -1725,4 +1864,162 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="7.33333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="24.2222222222222" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" ht="15.6" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="6"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="6"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added negative test for without select fans send vault media
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="4"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>email</t>
   </si>
@@ -167,6 +167,114 @@
   </si>
   <si>
     <t xml:space="preserve">a. Creator without vault media files </t>
+  </si>
+  <si>
+    <t>Scenario ID</t>
+  </si>
+  <si>
+    <t>Test Case Description</t>
+  </si>
+  <si>
+    <t>C-101</t>
+  </si>
+  <si>
+    <t>Creator tries to send without selecting vault file</t>
+  </si>
+  <si>
+    <t>C-102</t>
+  </si>
+  <si>
+    <t>Creator leaves message body empty (if required)</t>
+  </si>
+  <si>
+    <t>C-103</t>
+  </si>
+  <si>
+    <t>Creator selects invalid file format or corrupted vault item</t>
+  </si>
+  <si>
+    <t>C-104</t>
+  </si>
+  <si>
+    <t>Creator tries to send with no fan selected</t>
+  </si>
+  <si>
+    <t>C-105</t>
+  </si>
+  <si>
+    <t>Creator clicks "Send" with a disabled button (UI check)</t>
+  </si>
+  <si>
+    <t>C-106</t>
+  </si>
+  <si>
+    <t>Creator token/session expired while composing media</t>
+  </si>
+  <si>
+    <t>Boundary value</t>
+  </si>
+  <si>
+    <t>C-201</t>
+  </si>
+  <si>
+    <t>Send vault message to exactly 1 fan</t>
+  </si>
+  <si>
+    <t>C-202</t>
+  </si>
+  <si>
+    <t>Send vault message to max allowed fans (e.g., 1000)</t>
+  </si>
+  <si>
+    <t>C-203</t>
+  </si>
+  <si>
+    <t>Vault media title/message is 1 character long</t>
+  </si>
+  <si>
+    <t>C-204</t>
+  </si>
+  <si>
+    <t>Vault media message is exactly max allowed characters (e.g., 500)</t>
+  </si>
+  <si>
+    <t>C-205</t>
+  </si>
+  <si>
+    <t>Vault media message is 1 character over the limit – should fail</t>
+  </si>
+  <si>
+    <t>C-206</t>
+  </si>
+  <si>
+    <t>Uploading maximum allowed vault files in one message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exception Handling </t>
+  </si>
+  <si>
+    <t>C-301</t>
+  </si>
+  <si>
+    <t>Creator loses internet before sending – app gracefully handles</t>
+  </si>
+  <si>
+    <t>C-302</t>
+  </si>
+  <si>
+    <t>Creator closes tab midway – no partial/incomplete send on backend</t>
+  </si>
+  <si>
+    <t>C-303</t>
+  </si>
+  <si>
+    <t>Vault API fails mid-process – UI shows retry or fallback</t>
+  </si>
+  <si>
+    <t>C-304</t>
+  </si>
+  <si>
+    <t>Creator sends during live server maintenance – gets clear error</t>
   </si>
 </sst>
 </file>
@@ -833,7 +941,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -852,11 +960,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1452,47 +1566,47 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="22" t="s">
+    <row r="1" s="23" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="b">
+      <c r="C2" s="13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="11" t="b">
+      <c r="C3" s="13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11" t="b">
+      <c r="C4" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1524,46 +1638,46 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="22" t="s">
+    <row r="1" s="23" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="b">
+      <c r="C2" s="13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="11" t="b">
+      <c r="C3" s="13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="19"/>
+      <c r="C4" s="21"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1591,65 +1705,65 @@
     <col min="2" max="2" width="27.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="19.1111111111111" customWidth="1"/>
     <col min="4" max="4" width="35.5555555555556" customWidth="1"/>
-    <col min="5" max="5" width="20" style="16" customWidth="1"/>
-    <col min="7" max="7" width="28.3333333333333" style="16" customWidth="1"/>
+    <col min="5" max="5" width="20" style="18" customWidth="1"/>
+    <col min="7" max="7" width="28.3333333333333" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="17"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="G2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
-      <c r="A3" s="11"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="G3" s="19"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="11"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" s="20"/>
+      <c r="B7" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1679,38 +1793,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="13"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" ht="28" customHeight="1" spans="1:4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="11"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" ht="31" customHeight="1" spans="1:4">
-      <c r="A3" s="11"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="11"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:4">
-      <c r="A4" s="11"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="11"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1727,8 +1841,8 @@
   <sheetPr/>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1739,28 +1853,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" ht="57.6" spans="1:1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" ht="28.8" spans="1:2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" ht="28.8" spans="1:2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1869,10 +1983,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:D31"/>
+  <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1970,50 +2084,189 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="6"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="6"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="6"/>
-    </row>
-    <row r="21" spans="1:1">
+    <row r="15" spans="2:2">
+      <c r="B15" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" ht="28.8" spans="1:3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" ht="28.8" spans="1:3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" ht="43.2" spans="1:3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" ht="28.8" spans="1:3">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" ht="28.8" spans="1:3">
       <c r="A21"/>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" ht="43.2" spans="1:3">
       <c r="A22"/>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23"/>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24"/>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" ht="28.8" spans="1:3">
       <c r="A25"/>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" ht="28.8" spans="1:3">
       <c r="A26"/>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" ht="28.8" spans="1:3">
       <c r="A27"/>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" ht="43.2" spans="1:3">
       <c r="A28"/>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" ht="43.2" spans="1:3">
       <c r="A29"/>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" ht="43.2" spans="1:3">
       <c r="A30"/>
+      <c r="B30" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31"/>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" ht="43.2" spans="2:3">
+      <c r="B34" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" ht="43.2" spans="2:3">
+      <c r="B35" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" ht="28.8" spans="2:3">
+      <c r="B36" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" ht="43.2" spans="2:3">
+      <c r="B37" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated the vault media send negative test
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -166,7 +166,7 @@
     <t xml:space="preserve">a. Creator Send vault media files </t>
   </si>
   <si>
-    <t xml:space="preserve">a. Creator without vault media files </t>
+    <t>a. Creator tries to send without selecting vault file</t>
   </si>
   <si>
     <t>Scenario ID</t>
@@ -1985,15 +1985,15 @@
   <sheetPr/>
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="7.33333333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="24.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="42.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="33.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" ht="15.6" spans="1:4">
@@ -2115,7 +2115,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" ht="43.2" spans="1:3">
+    <row r="19" ht="28.8" spans="1:3">
       <c r="A19" s="8"/>
       <c r="B19" s="9" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Added new massMsgFun() test and Po class
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="5"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>email</t>
   </si>
@@ -169,7 +169,7 @@
     <t>a. Creator tries to send without selecting vault file</t>
   </si>
   <si>
-    <t>Scenario ID</t>
+    <t>Test Scenario ID</t>
   </si>
   <si>
     <t>Test Case Description</t>
@@ -184,33 +184,9 @@
     <t>C-102</t>
   </si>
   <si>
-    <t>Creator leaves message body empty (if required)</t>
-  </si>
-  <si>
-    <t>C-103</t>
-  </si>
-  <si>
-    <t>Creator selects invalid file format or corrupted vault item</t>
-  </si>
-  <si>
-    <t>C-104</t>
-  </si>
-  <si>
     <t>Creator tries to send with no fan selected</t>
   </si>
   <si>
-    <t>C-105</t>
-  </si>
-  <si>
-    <t>Creator clicks "Send" with a disabled button (UI check)</t>
-  </si>
-  <si>
-    <t>C-106</t>
-  </si>
-  <si>
-    <t>Creator token/session expired while composing media</t>
-  </si>
-  <si>
     <t>Boundary value</t>
   </si>
   <si>
@@ -256,7 +232,7 @@
     <t>C-301</t>
   </si>
   <si>
-    <t>Creator loses internet before sending – app gracefully handles</t>
+    <t>Creator loses internet before sending vault media – app gracefully handles</t>
   </si>
   <si>
     <t>C-302</t>
@@ -941,7 +917,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -968,6 +944,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1566,47 +1545,47 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="23" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="24" t="s">
+    <row r="1" s="24" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="b">
+      <c r="C2" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="b">
+      <c r="C3" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="13" t="b">
+      <c r="C4" s="14" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1638,46 +1617,46 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="23" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="24" t="s">
+    <row r="1" s="24" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="b">
+      <c r="C2" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13" t="b">
+      <c r="C3" s="14" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="21"/>
+      <c r="C4" s="22"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1705,65 +1684,65 @@
     <col min="2" max="2" width="27.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="19.1111111111111" customWidth="1"/>
     <col min="4" max="4" width="35.5555555555556" customWidth="1"/>
-    <col min="5" max="5" width="20" style="18" customWidth="1"/>
-    <col min="7" max="7" width="28.3333333333333" style="18" customWidth="1"/>
+    <col min="5" max="5" width="20" style="19" customWidth="1"/>
+    <col min="7" max="7" width="28.3333333333333" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="19"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="G2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
-      <c r="A3" s="13"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="G3" s="21"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="13"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" s="22"/>
+      <c r="B7" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1793,38 +1772,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" ht="28" customHeight="1" spans="1:4">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" ht="31" customHeight="1" spans="1:4">
-      <c r="A3" s="13"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="13"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:4">
-      <c r="A4" s="13"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="13"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1858,23 +1837,23 @@
       </c>
     </row>
     <row r="2" ht="57.6" spans="1:1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" ht="28.8" spans="1:2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" ht="28.8" spans="1:2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1985,15 +1964,15 @@
   <sheetPr/>
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="7.33333333333333" style="1" customWidth="1"/>
     <col min="2" max="2" width="42.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="33.5555555555556" customWidth="1"/>
+    <col min="3" max="3" width="60.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" ht="15.6" spans="1:4">
@@ -2097,64 +2076,47 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" ht="28.8" spans="1:3">
+    <row r="17" spans="1:3">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" ht="28.8" spans="1:3">
+    <row r="18" spans="1:3">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" ht="28.8" spans="1:3">
+    <row r="19" spans="1:3">
       <c r="A19" s="8"/>
-      <c r="B19" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" ht="28.8" spans="1:3">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="8"/>
-      <c r="B20" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" ht="28.8" spans="1:3">
+      <c r="B20" s="9"/>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21"/>
-      <c r="B21" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" ht="43.2" spans="1:3">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22"/>
-      <c r="B22" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23"/>
       <c r="B23" s="6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2166,58 +2128,58 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" ht="28.8" spans="1:3">
+    <row r="25" spans="1:3">
       <c r="A25"/>
       <c r="B25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" ht="28.8" spans="1:3">
+        <v>45</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" ht="19" customHeight="1" spans="1:3">
       <c r="A26"/>
       <c r="B26" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" ht="28.8" spans="1:3">
+        <v>47</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27"/>
       <c r="B27" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" ht="43.2" spans="1:3">
+        <v>49</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28"/>
       <c r="B28" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" ht="43.2" spans="1:3">
+        <v>51</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" ht="18" customHeight="1" spans="1:3">
       <c r="A29"/>
       <c r="B29" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" ht="43.2" spans="1:3">
+        <v>53</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30"/>
       <c r="B30" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>64</v>
+        <v>55</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:1">
@@ -2225,7 +2187,7 @@
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:3">
@@ -2236,36 +2198,36 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" ht="43.2" spans="2:3">
+    <row r="34" ht="15" customHeight="1" spans="2:3">
       <c r="B34" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" ht="43.2" spans="2:3">
+        <v>58</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
       <c r="B35" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" ht="28.8" spans="2:3">
+        <v>60</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" ht="19" customHeight="1" spans="2:3">
       <c r="B36" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" ht="43.2" spans="2:3">
+        <v>62</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
       <c r="B37" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>73</v>
+        <v>64</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the massmsgFun tests
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -169,7 +169,7 @@
     <t>a. Creator tries to send without selecting vault file</t>
   </si>
   <si>
-    <t>Test Scenario ID</t>
+    <t>Scenario ID</t>
   </si>
   <si>
     <t>Test Case Description</t>
@@ -1964,8 +1964,8 @@
   <sheetPr/>
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
Update the signin Test
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="5"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
   <si>
     <t>email</t>
   </si>
@@ -65,7 +65,13 @@
     <t>user@</t>
   </si>
   <si>
-    <t>Short@123</t>
+    <t>ValidPass@1</t>
+  </si>
+  <si>
+    <t>user11@example.c</t>
+  </si>
+  <si>
+    <t>ValidPass@</t>
   </si>
   <si>
     <t>CreatorEmail</t>
@@ -917,7 +923,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -954,9 +960,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -966,15 +969,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -987,17 +984,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1007,7 +998,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1535,7 +1526,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1545,47 +1536,47 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="24" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="25" t="s">
+    <row r="1" s="20" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14" t="b">
+      <c r="C2" s="13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="b">
+      <c r="C3" s="13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="14" t="b">
+      <c r="C4" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1604,65 +1595,93 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="17.8888888888889" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="24" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="25" t="s">
+    <row r="1" s="20" customFormat="1" ht="15.6" spans="1:3">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14" t="b">
+      <c r="C2" s="13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="14" t="b">
+      <c r="C4" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:3">
-      <c r="C4" s="22"/>
-    </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="13" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="ValidPass@123"/>
-    <hyperlink ref="B3" r:id="rId2" display="Short@123"/>
-    <hyperlink ref="A2" r:id="rId3" display="user11@example.com" tooltip="mailto:user11@example.com"/>
+    <hyperlink ref="A2" r:id="rId2" display="user11@example.com" tooltip="mailto:user11@example.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="user11@example.com" tooltip="mailto:user11@example.com"/>
+    <hyperlink ref="B4" r:id="rId3" display="ValidPass@1" tooltip="mailto:ValidPass@1"/>
+    <hyperlink ref="A5" r:id="rId4" display="user11@example.c" tooltip="mailto:user11@example.c"/>
+    <hyperlink ref="B5" r:id="rId3" display="ValidPass@" tooltip="mailto:ValidPass@1"/>
+    <hyperlink ref="B3" r:id="rId1" display="ValidPass@123"/>
+    <hyperlink ref="B6" r:id="rId3" display="ValidPass@" tooltip="mailto:ValidPass@1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1684,65 +1703,65 @@
     <col min="2" max="2" width="27.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="19.1111111111111" customWidth="1"/>
     <col min="4" max="4" width="35.5555555555556" customWidth="1"/>
-    <col min="5" max="5" width="20" style="19" customWidth="1"/>
-    <col min="7" max="7" width="28.3333333333333" style="19" customWidth="1"/>
+    <col min="5" max="5" width="20" style="16" customWidth="1"/>
+    <col min="7" max="7" width="28.3333333333333" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="20"/>
+      <c r="C1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
-      <c r="A2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" ht="44" customHeight="1" spans="1:7">
-      <c r="A3" s="14"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="G3" s="22"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="14"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" s="23"/>
+      <c r="B7" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1772,38 +1791,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="16"/>
+      <c r="B1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" ht="28" customHeight="1" spans="1:4">
-      <c r="A2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="14"/>
+      <c r="A2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" ht="31" customHeight="1" spans="1:4">
-      <c r="A3" s="14"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" ht="30" customHeight="1" spans="1:4">
-      <c r="A4" s="14"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1833,33 +1852,33 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" ht="57.6" spans="1:1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" ht="302.4" spans="1:1">
       <c r="A2" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" ht="28.8" spans="1:2">
-      <c r="A5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="28.8" spans="1:2">
-      <c r="A6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="13" t="s">
+    <row r="6" ht="43.2" spans="1:2">
+      <c r="A6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" ht="15.6" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1867,16 +1886,16 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1884,7 +1903,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1892,7 +1911,7 @@
     <row r="14" spans="1:4">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1914,7 +1933,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1922,7 +1941,7 @@
     <row r="18" spans="1:4">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1964,7 +1983,7 @@
   <sheetPr/>
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1977,7 +1996,7 @@
   <sheetData>
     <row r="2" ht="15.6" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1985,16 +2004,16 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2002,7 +2021,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2010,7 +2029,7 @@
     <row r="5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2032,7 +2051,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2040,7 +2059,7 @@
     <row r="9" spans="1:4">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2065,33 +2084,33 @@
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2116,70 +2135,70 @@
     <row r="23" spans="1:2">
       <c r="A23"/>
       <c r="B23" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24"/>
       <c r="B24" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25"/>
       <c r="B25" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" ht="19" customHeight="1" spans="1:3">
       <c r="A26"/>
       <c r="B26" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27"/>
       <c r="B27" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28"/>
       <c r="B28" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:3">
       <c r="A29"/>
       <c r="B29" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30"/>
       <c r="B30" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:1">
@@ -2187,47 +2206,47 @@
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="2:3">
       <c r="B34" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" ht="19" customHeight="1" spans="2:3">
       <c r="B36" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the signup tests
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
   <si>
     <t>email</t>
   </si>
@@ -43,13 +43,13 @@
     <t>isValid</t>
   </si>
   <si>
-    <t>rohan.kapse.iic.0148+RockHero@gmail.com</t>
+    <t>rohan.kapse.iic.0148+RockMetro@gmail.com</t>
   </si>
   <si>
     <t>ValidPass@123</t>
   </si>
   <si>
-    <t xml:space="preserve">rohan.kapse.iic.0148+RockStar3@gmail.com
+    <t xml:space="preserve">rohan.kapse.iic.0148+RockStar3@gmai
 </t>
   </si>
   <si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>rohan.kapse.iic.0148+RockHeroNoOne@gmail.com</t>
+  </si>
+  <si>
+    <t>rohan.kapse.iic.0148+RockHeroNotwo@gmail.com</t>
   </si>
   <si>
     <t>user11@example.com</t>
@@ -1523,13 +1529,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="33.3333333333333" customWidth="1"/>
     <col min="2" max="2" width="17.8888888888889" customWidth="1"/>
@@ -1558,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="43.2" spans="1:3">
+    <row r="3" ht="28.8" spans="1:3">
       <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
@@ -1566,7 +1572,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1577,6 +1583,35 @@
         <v>7</v>
       </c>
       <c r="C4" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="28.8" spans="1:3">
+      <c r="A5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="28.8" spans="1:3">
+      <c r="A7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1584,8 +1619,10 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
     <hyperlink ref="A4" r:id="rId2" display="another@example.com" tooltip="mailto:another@example.com"/>
-    <hyperlink ref="A3" r:id="rId3" display="rohan.kapse.iic.0148+RockStar3@gmail.com&#10;"/>
+    <hyperlink ref="A3" r:id="rId3" display="rohan.kapse.iic.0148+RockStar3@gmai&#10;"/>
     <hyperlink ref="B3" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="B5" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="B6" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1597,8 +1634,8 @@
   <sheetPr/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
@@ -1621,7 +1658,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>4</v>
@@ -1632,7 +1669,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>4</v>
@@ -1643,10 +1680,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="13" t="b">
         <v>0</v>
@@ -1654,10 +1691,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="13" t="b">
         <v>0</v>
@@ -1666,7 +1703,7 @@
     <row r="6" spans="1:3">
       <c r="A6" s="13"/>
       <c r="B6" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" s="13" t="b">
         <v>0</v>
@@ -1709,25 +1746,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G1" s="17"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
       <c r="A2" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="13"/>
@@ -1792,22 +1829,22 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" ht="28" customHeight="1" spans="1:4">
       <c r="A2" s="13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="13"/>
@@ -1852,17 +1889,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" ht="302.4" spans="1:1">
       <c r="A2" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>4</v>
@@ -1870,7 +1907,7 @@
     </row>
     <row r="6" ht="43.2" spans="1:2">
       <c r="A6" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>4</v>
@@ -1878,7 +1915,7 @@
     </row>
     <row r="11" ht="15.6" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1886,16 +1923,16 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1903,7 +1940,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1911,7 +1948,7 @@
     <row r="14" spans="1:4">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1933,7 +1970,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1941,7 +1978,7 @@
     <row r="18" spans="1:4">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1996,7 +2033,7 @@
   <sheetData>
     <row r="2" ht="15.6" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2004,16 +2041,16 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2021,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2029,7 +2066,7 @@
     <row r="5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2051,7 +2088,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2059,7 +2096,7 @@
     <row r="9" spans="1:4">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2084,33 +2121,33 @@
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2135,70 +2172,70 @@
     <row r="23" spans="1:2">
       <c r="A23"/>
       <c r="B23" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24"/>
       <c r="B24" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25"/>
       <c r="B25" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" ht="19" customHeight="1" spans="1:3">
       <c r="A26"/>
       <c r="B26" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27"/>
       <c r="B27" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28"/>
       <c r="B28" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:3">
       <c r="A29"/>
       <c r="B29" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30"/>
       <c r="B30" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:1">
@@ -2206,47 +2243,47 @@
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="2:3">
       <c r="B34" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" ht="19" customHeight="1" spans="2:3">
       <c r="B36" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upadte signup test and add Signup test for cretor
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="signup_data" sheetId="1" r:id="rId1"/>
-    <sheet name="signin_data" sheetId="2" r:id="rId2"/>
-    <sheet name="massMsgSend_Data" sheetId="3" r:id="rId3"/>
-    <sheet name="users_LoginData" sheetId="4" r:id="rId4"/>
-    <sheet name="massMessage_TestScenarios" sheetId="5" r:id="rId5"/>
-    <sheet name="massVaultMedia_TestScenarios" sheetId="6" r:id="rId6"/>
+    <sheet name="signupCreator_data" sheetId="7" r:id="rId2"/>
+    <sheet name="signin_data" sheetId="2" r:id="rId3"/>
+    <sheet name="massMsgSend_Data" sheetId="3" r:id="rId4"/>
+    <sheet name="users_LoginData" sheetId="4" r:id="rId5"/>
+    <sheet name="massMessage_TestScenarios" sheetId="5" r:id="rId6"/>
+    <sheet name="massVaultMedia_TestScenarios" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
   <si>
     <t>email</t>
   </si>
@@ -43,7 +44,7 @@
     <t>isValid</t>
   </si>
   <si>
-    <t>rohan.kapse.iic.0148+RockMetro@gmail.com</t>
+    <t>rohan.kapse.iic.0148+RockMetroStar@gmail.com</t>
   </si>
   <si>
     <t>ValidPass@123</t>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t>rohan.kapse.iic.0148+RockHeroNotwo@gmail.com</t>
+  </si>
+  <si>
+    <t>rohan.kapse.iic.0148+KieronP@gmail.com</t>
   </si>
   <si>
     <t>user11@example.com</t>
@@ -1531,8 +1535,8 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -1630,6 +1634,109 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="20.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" spans="1:3">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="34" customHeight="1" spans="1:3">
+      <c r="A2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="28" customHeight="1" spans="1:3">
+      <c r="A3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="28" customHeight="1" spans="1:3">
+      <c r="A4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="43.2" spans="1:3">
+      <c r="A5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" ht="22" customHeight="1" spans="1:3">
+      <c r="A7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="A4" r:id="rId2" display="another@example.com" tooltip="mailto:another@example.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="rohan.kapse.iic.0148+RockStar3@gmai&#10;"/>
+    <hyperlink ref="B3" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="B5" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="B6" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C6"/>
@@ -1658,7 +1765,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>4</v>
@@ -1669,7 +1776,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>4</v>
@@ -1680,10 +1787,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="13" t="b">
         <v>0</v>
@@ -1691,10 +1798,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="13" t="b">
         <v>0</v>
@@ -1703,7 +1810,7 @@
     <row r="6" spans="1:3">
       <c r="A6" s="13"/>
       <c r="B6" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="13" t="b">
         <v>0</v>
@@ -1725,7 +1832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:G7"/>
@@ -1746,25 +1853,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="17"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
       <c r="A2" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="13"/>
@@ -1810,7 +1917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D4"/>
@@ -1829,22 +1936,22 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" ht="28" customHeight="1" spans="1:4">
       <c r="A2" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="13"/>
@@ -1871,7 +1978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D21"/>
@@ -1889,17 +1996,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" ht="302.4" spans="1:1">
       <c r="A2" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>4</v>
@@ -1907,7 +2014,7 @@
     </row>
     <row r="6" ht="43.2" spans="1:2">
       <c r="A6" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>4</v>
@@ -1915,7 +2022,7 @@
     </row>
     <row r="11" ht="15.6" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1923,16 +2030,16 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1940,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1948,7 +2055,7 @@
     <row r="14" spans="1:4">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1970,7 +2077,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1978,7 +2085,7 @@
     <row r="18" spans="1:4">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2015,7 +2122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A2:D37"/>
@@ -2033,7 +2140,7 @@
   <sheetData>
     <row r="2" ht="15.6" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2041,16 +2148,16 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2058,7 +2165,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2066,7 +2173,7 @@
     <row r="5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2088,7 +2195,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2096,7 +2203,7 @@
     <row r="9" spans="1:4">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2121,33 +2228,33 @@
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2172,70 +2279,70 @@
     <row r="23" spans="1:2">
       <c r="A23"/>
       <c r="B23" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24"/>
       <c r="B24" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25"/>
       <c r="B25" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" ht="19" customHeight="1" spans="1:3">
       <c r="A26"/>
       <c r="B26" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27"/>
       <c r="B27" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28"/>
       <c r="B28" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:3">
       <c r="A29"/>
       <c r="B29" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30"/>
       <c r="B30" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:1">
@@ -2243,47 +2350,47 @@
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="2:3">
       <c r="B34" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" ht="19" customHeight="1" spans="2:3">
       <c r="B36" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the yml files for upadetd signup test and massmsgfun test
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="1"/>
+    <workbookView windowWidth="10511" windowHeight="3096" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="signupFan_data" sheetId="1" r:id="rId1"/>
@@ -1638,8 +1638,8 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -1741,8 +1741,8 @@
   <sheetPr/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
Update the vault media parallel test and method of recived vaultmedia
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10511" windowHeight="3096" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9000" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="signupFan_data" sheetId="1" r:id="rId1"/>
@@ -1638,8 +1638,8 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -1693,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" ht="43.2" spans="1:3">
+    <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
@@ -1741,7 +1741,7 @@
   <sheetPr/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update the signup test
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="signupFan_data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
+  <si>
+    <t>Username</t>
+  </si>
   <si>
     <t>email</t>
   </si>
@@ -44,29 +47,65 @@
     <t>isValid</t>
   </si>
   <si>
+    <t>ryankite</t>
+  </si>
+  <si>
     <t>rohan.kapse.iic.0148+RockMetroStarBoys@gmail.com</t>
   </si>
   <si>
     <t>ValidPass@123</t>
+  </si>
+  <si>
+    <t>dyankite</t>
   </si>
   <si>
     <t xml:space="preserve">rohan.kapse.iic.0148+RockStar3@gmai
 </t>
   </si>
   <si>
+    <t>hyankite</t>
+  </si>
+  <si>
     <t>another@example.com</t>
   </si>
   <si>
     <t>pass</t>
   </si>
   <si>
+    <t>gyanskite</t>
+  </si>
+  <si>
     <t>rohan.kapse.iic.0148+RockHeroNoOne@gmail.com</t>
   </si>
   <si>
+    <t>pyankite</t>
+  </si>
+  <si>
+    <t>zyankite</t>
+  </si>
+  <si>
     <t>rohan.kapse.iic.0148+RockHeroNotwo@gmail.com</t>
   </si>
   <si>
+    <t>ryanstar</t>
+  </si>
+  <si>
     <t>rohan.kapse.iic.0148+KieronPollardOne@gmail.com</t>
+  </si>
+  <si>
+    <t>dyanstar</t>
+  </si>
+  <si>
+    <t>hyanstar</t>
+  </si>
+  <si>
+    <t>gyanstar</t>
+  </si>
+  <si>
+    <t>pyanstar</t>
+  </si>
+  <si>
+    <t>zyanstar</t>
   </si>
   <si>
     <t>user11@example.com</t>
@@ -933,7 +972,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -999,6 +1038,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1533,21 +1587,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="33.3333333333333" customWidth="1"/>
-    <col min="2" max="2" width="17.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="1" max="1" width="15.1111111111111" customWidth="1"/>
+    <col min="2" max="2" width="33.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="17.8888888888889" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="1" ht="15.6" spans="1:3">
-      <c r="A1" s="21" t="s">
+    <row r="1" s="20" customFormat="1" ht="15.6" spans="1:4">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -1556,77 +1611,98 @@
       <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" ht="28.8" spans="1:3">
-      <c r="A2" s="13" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+    </row>
+    <row r="2" ht="28.8" spans="1:4">
+      <c r="A2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="b">
+      <c r="B2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="28.8" spans="1:3">
-      <c r="A3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="13" t="b">
+    <row r="3" ht="28.8" spans="1:4">
+      <c r="A3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" ht="28.8" spans="1:4">
+      <c r="A5" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="13" t="b">
+      <c r="D5" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" ht="28.8" spans="1:3">
-      <c r="A5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="13" t="b">
+    <row r="6" spans="1:4">
+      <c r="A6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="28.8" spans="1:3">
-      <c r="A7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13" t="b">
+    <row r="7" ht="28.8" spans="1:4">
+      <c r="A7" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
-    <hyperlink ref="A4" r:id="rId2" display="another@example.com" tooltip="mailto:another@example.com"/>
-    <hyperlink ref="A3" r:id="rId3" display="rohan.kapse.iic.0148+RockStar3@gmai&#10;"/>
-    <hyperlink ref="B3" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
-    <hyperlink ref="B5" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
-    <hyperlink ref="B6" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="C2" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="B4" r:id="rId2" display="another@example.com" tooltip="mailto:another@example.com"/>
+    <hyperlink ref="B3" r:id="rId3" display="rohan.kapse.iic.0148+RockStar3@gmai&#10;"/>
+    <hyperlink ref="C3" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="C5" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="C6" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1636,21 +1712,22 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="20.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="1" max="1" width="13.7777777777778" style="22" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="3" max="3" width="20.7777777777778" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:3">
-      <c r="A1" s="21" t="s">
+    <row r="1" ht="15" customHeight="1" spans="1:4">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -1659,77 +1736,98 @@
       <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" ht="34" customHeight="1" spans="1:3">
-      <c r="A2" s="13" t="s">
+      <c r="D1" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" ht="34" customHeight="1" spans="1:4">
+      <c r="A2" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="28" customHeight="1" spans="1:4">
+      <c r="A3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" ht="28" customHeight="1" spans="1:4">
+      <c r="A4" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" ht="28" customHeight="1" spans="1:3">
-      <c r="A3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="13" t="b">
+      <c r="C4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" ht="28" customHeight="1" spans="1:3">
-      <c r="A4" s="13" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="13" t="b">
+      <c r="D5" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="13" t="b">
+    <row r="6" spans="1:4">
+      <c r="A6" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="22" customHeight="1" spans="1:3">
-      <c r="A7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13" t="b">
+    <row r="7" ht="22" customHeight="1" spans="1:4">
+      <c r="A7" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
-    <hyperlink ref="A4" r:id="rId2" display="another@example.com" tooltip="mailto:another@example.com"/>
-    <hyperlink ref="A3" r:id="rId3" display="rohan.kapse.iic.0148+RockStar3@gmai&#10;"/>
-    <hyperlink ref="B3" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
-    <hyperlink ref="B5" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
-    <hyperlink ref="B6" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="C2" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="B4" r:id="rId2" display="another@example.com" tooltip="mailto:another@example.com"/>
+    <hyperlink ref="B3" r:id="rId3" display="rohan.kapse.iic.0148+RockStar3@gmai&#10;"/>
+    <hyperlink ref="C3" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="C5" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
+    <hyperlink ref="C6" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1742,7 +1840,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
@@ -1754,21 +1852,21 @@
   <sheetData>
     <row r="1" s="20" customFormat="1" ht="15.6" spans="1:3">
       <c r="A1" s="21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="13" t="b">
         <v>1</v>
@@ -1776,10 +1874,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="13" t="b">
         <v>0</v>
@@ -1787,10 +1885,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C4" s="13" t="b">
         <v>0</v>
@@ -1798,10 +1896,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C5" s="13" t="b">
         <v>0</v>
@@ -1810,7 +1908,7 @@
     <row r="6" spans="1:3">
       <c r="A6" s="13"/>
       <c r="B6" s="12" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C6" s="13" t="b">
         <v>0</v>
@@ -1818,7 +1916,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="ValidPass@123"/>
+    <hyperlink ref="B2" r:id="rId1" display="ValidPass@123" tooltip="mailto:ValidPass@123"/>
     <hyperlink ref="A2" r:id="rId2" display="user11@example.com" tooltip="mailto:user11@example.com"/>
     <hyperlink ref="A4" r:id="rId2" display="user11@example.com" tooltip="mailto:user11@example.com"/>
     <hyperlink ref="B4" r:id="rId3" display="ValidPass@1" tooltip="mailto:ValidPass@1"/>
@@ -1853,25 +1951,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="14" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G1" s="17"/>
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:7">
       <c r="A2" s="13" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="13"/>
@@ -1936,22 +2034,22 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="14" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" ht="28" customHeight="1" spans="1:4">
       <c r="A2" s="13" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="13"/>
@@ -1984,7 +2082,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1996,33 +2094,33 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" ht="302.4" spans="1:1">
       <c r="A2" s="11" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" ht="43.2" spans="1:2">
       <c r="A6" s="13" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" ht="15.6" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2030,16 +2128,16 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2047,7 +2145,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2055,7 +2153,7 @@
     <row r="14" spans="1:4">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2077,7 +2175,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2085,7 +2183,7 @@
     <row r="18" spans="1:4">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2140,7 +2238,7 @@
   <sheetData>
     <row r="2" ht="15.6" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2148,16 +2246,16 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2165,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2173,7 +2271,7 @@
     <row r="5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2195,7 +2293,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2203,7 +2301,7 @@
     <row r="9" spans="1:4">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2228,33 +2326,33 @@
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="6" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" s="7" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2279,70 +2377,70 @@
     <row r="23" spans="1:2">
       <c r="A23"/>
       <c r="B23" s="6" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24"/>
       <c r="B24" s="7" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25"/>
       <c r="B25" s="9" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" ht="19" customHeight="1" spans="1:3">
       <c r="A26"/>
       <c r="B26" s="9" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27"/>
       <c r="B27" s="9" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28"/>
       <c r="B28" s="9" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" ht="18" customHeight="1" spans="1:3">
       <c r="A29"/>
       <c r="B29" s="9" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30"/>
       <c r="B30" s="9" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:1">
@@ -2350,47 +2448,47 @@
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="6" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="7" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="2:3">
       <c r="B34" s="9" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="9" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" ht="19" customHeight="1" spans="2:3">
       <c r="B36" s="9" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" s="9" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the chatpage and parallel mass msg test
</commit_message>
<xml_diff>
--- a/data/testData.xlsx
+++ b/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="signupFan_data" sheetId="1" r:id="rId1"/>
@@ -972,7 +972,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1039,19 +1039,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1602,7 +1590,7 @@
   </cols>
   <sheetData>
     <row r="1" s="20" customFormat="1" ht="15.6" spans="1:4">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -1616,7 +1604,7 @@
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:4">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -1630,7 +1618,7 @@
       </c>
     </row>
     <row r="3" ht="28.8" spans="1:4">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -1644,7 +1632,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -1658,7 +1646,7 @@
       </c>
     </row>
     <row r="5" ht="28.8" spans="1:4">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1672,7 +1660,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="13"/>
@@ -1684,7 +1672,7 @@
       </c>
     </row>
     <row r="7" ht="28.8" spans="1:4">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -1714,20 +1702,20 @@
   <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="13.7777777777778" style="22" customWidth="1"/>
+    <col min="1" max="1" width="13.7777777777778" style="1" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="20.7777777777778" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" spans="1:4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -1741,7 +1729,7 @@
       </c>
     </row>
     <row r="2" ht="34" customHeight="1" spans="1:4">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -1755,7 +1743,7 @@
       </c>
     </row>
     <row r="3" ht="28" customHeight="1" spans="1:4">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -1769,7 +1757,7 @@
       </c>
     </row>
     <row r="4" ht="28" customHeight="1" spans="1:4">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -1783,7 +1771,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -1797,7 +1785,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="13"/>
@@ -1809,7 +1797,7 @@
       </c>
     </row>
     <row r="7" ht="22" customHeight="1" spans="1:4">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -2020,8 +2008,8 @@
   <sheetPr/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="3"/>

</xml_diff>